<commit_message>
updated readme, updated file name
</commit_message>
<xml_diff>
--- a/excel_docs/in_progress.xlsx
+++ b/excel_docs/in_progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/648742649a6f8c0c/Documents/GitHub/highlight_excels/excel_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{DC91B701-E484-4F3A-84FB-8711E1D2FAE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F4B28A5-ABD4-4777-9B9C-8D20A6C7BAB1}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{DC91B701-E484-4F3A-84FB-8711E1D2FAE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64727BA3-1553-49B1-8685-1229D2BFEF5B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3C6329DF-4F8C-4069-8EEF-F5CC61BABC37}"/>
   </bookViews>
@@ -134,9 +134,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>ISBNs (kinda)</t>
-  </si>
-  <si>
     <t>books</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>authors</t>
+  </si>
+  <si>
+    <t>ISBNs</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,13 +548,13 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>0</v>
@@ -797,10 +797,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>